<commit_message>
Refactored things to facilitate filtering
</commit_message>
<xml_diff>
--- a/OpenxmlConsoleApplication/bin/Debug/O&M_Copy.xlsx
+++ b/OpenxmlConsoleApplication/bin/Debug/O&M_Copy.xlsx
@@ -23,7 +23,7 @@
     <x:sheet name="Total Influent" sheetId="16" r:id="rId9"/>
     <x:sheet name="Weekly Inj_Rates" sheetId="8" r:id="rId10"/>
     <x:sheet name="Weekly Ext_Rates" sheetId="9" r:id="rId11"/>
-    <x:sheet name="records" sheetId="17" r:id="Rab139b6fbe354c81"/>
+    <x:sheet name="records" sheetId="17" r:id="Rc6c913541d714057"/>
   </x:sheets>
   <x:definedNames>
     <x:definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'RAW Data_all'!$A$1:$D$770</x:definedName>
@@ -73094,10 +73094,10 @@
         <x:v>42169</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>10.7360982510288</x:v>
+        <x:v>2.00694444444444</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>75919</x:v>
+        <x:v>14450</x:v>
       </x:c>
     </x:row>
     <x:row r="3">
@@ -73108,10 +73108,10 @@
         <x:v>42176</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>48.846875</x:v>
+        <x:v>6.86458333333333</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>216598</x:v>
+        <x:v>34220</x:v>
       </x:c>
     </x:row>
     <x:row r="4">
@@ -73122,10 +73122,10 @@
         <x:v>42183</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>58.5833333333333</x:v>
+        <x:v>10.7795138888889</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>554038</x:v>
+        <x:v>96310</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
@@ -73136,10 +73136,10 @@
         <x:v>42197</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>21.7322916666667</x:v>
+        <x:v>4.09027777777778</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>679216</x:v>
+        <x:v>119870</x:v>
       </x:c>
     </x:row>
     <x:row r="6">
@@ -73150,10 +73150,10 @@
         <x:v>42204</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>36.3551388888889</x:v>
+        <x:v>5.33611111111111</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>940973</x:v>
+        <x:v>158290</x:v>
       </x:c>
     </x:row>
     <x:row r="7">
@@ -73164,10 +73164,10 @@
         <x:v>42211</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>28.3994791666667</x:v>
+        <x:v>2.84548611111111</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>1104554</x:v>
+        <x:v>174680</x:v>
       </x:c>
     </x:row>
     <x:row r="8">
@@ -73178,10 +73178,10 @@
         <x:v>42218</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>19.3518055555556</x:v>
+        <x:v>3.50416666666667</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>1237800</x:v>
+        <x:v>199910</x:v>
       </x:c>
     </x:row>
     <x:row r="9">
@@ -73192,10 +73192,10 @@
         <x:v>42225</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>57.1697172619048</x:v>
+        <x:v>11.6510416666667</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>1544237</x:v>
+        <x:v>267020</x:v>
       </x:c>
     </x:row>
     <x:row r="10">
@@ -73206,10 +73206,10 @@
         <x:v>42232</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>36.8486111111111</x:v>
+        <x:v>9.02430555555556</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>1756485</x:v>
+        <x:v>319000</x:v>
       </x:c>
     </x:row>
     <x:row r="11">
@@ -73220,10 +73220,10 @@
         <x:v>42239</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>35.9184027777778</x:v>
+        <x:v>3.02430555555556</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>1963375</x:v>
+        <x:v>336420</x:v>
       </x:c>
     </x:row>
     <x:row r="12">
@@ -73234,10 +73234,10 @@
         <x:v>42246</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>52.9684027777778</x:v>
+        <x:v>10.6875</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>2115924</x:v>
+        <x:v>367200</x:v>
       </x:c>
     </x:row>
     <x:row r="13">
@@ -73248,10 +73248,10 @@
         <x:v>42253</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>59.1840277777778</x:v>
+        <x:v>12.1510416666667</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>2456824</x:v>
+        <x:v>437190</x:v>
       </x:c>
     </x:row>
     <x:row r="14">
@@ -73262,10 +73262,10 @@
         <x:v>42260</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>42.6241319444444</x:v>
+        <x:v>6.72048611111111</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>2702339</x:v>
+        <x:v>475900</x:v>
       </x:c>
     </x:row>
     <x:row r="15">
@@ -73276,10 +73276,10 @@
         <x:v>42267</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>24.2868055555556</x:v>
+        <x:v>3.25347222222222</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>2772285</x:v>
+        <x:v>485270</x:v>
       </x:c>
     </x:row>
     <x:row r="16">
@@ -73290,10 +73290,10 @@
         <x:v>42274</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>56.0972222222222</x:v>
+        <x:v>14.8819444444444</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>3095405</x:v>
+        <x:v>570990</x:v>
       </x:c>
     </x:row>
     <x:row r="17">
@@ -73304,10 +73304,10 @@
         <x:v>42281</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>53.6204861111111</x:v>
+        <x:v>12.4184027777778</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>3404259</x:v>
+        <x:v>642520</x:v>
       </x:c>
     </x:row>
     <x:row r="18">
@@ -73318,10 +73318,10 @@
         <x:v>42288</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>48.3909722222222</x:v>
+        <x:v>9.578125</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>3682991</x:v>
+        <x:v>697690</x:v>
       </x:c>
     </x:row>
     <x:row r="19">
@@ -73332,10 +73332,10 @@
         <x:v>42295</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>48.8590277777778</x:v>
+        <x:v>9.09722222222222</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>3964419</x:v>
+        <x:v>750090</x:v>
       </x:c>
     </x:row>
     <x:row r="20">
@@ -73346,10 +73346,10 @@
         <x:v>42302</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>60.3446180555556</x:v>
+        <x:v>13.4930555555556</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>4312004</x:v>
+        <x:v>827810</x:v>
       </x:c>
     </x:row>
     <x:row r="21">
@@ -73360,10 +73360,10 @@
         <x:v>42309</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>52.2800347222222</x:v>
+        <x:v>10.4861111111111</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>4582937</x:v>
+        <x:v>858010</x:v>
       </x:c>
     </x:row>
     <x:row r="22">
@@ -73374,10 +73374,10 @@
         <x:v>42316</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>53.0352430555556</x:v>
+        <x:v>9.95659722222222</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>4888420</x:v>
+        <x:v>915360</x:v>
       </x:c>
     </x:row>
     <x:row r="23">
@@ -73388,10 +73388,10 @@
         <x:v>42323</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>71.4979166666667</x:v>
+        <x:v>8.88888888888889</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>5300248</x:v>
+        <x:v>966560</x:v>
       </x:c>
     </x:row>
     <x:row r="24">
@@ -73402,10 +73402,10 @@
         <x:v>42330</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>54.0086805555555</x:v>
+        <x:v>11.4340277777778</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>5455793</x:v>
+        <x:v>999490</x:v>
       </x:c>
     </x:row>
     <x:row r="25">
@@ -73416,10 +73416,10 @@
         <x:v>42337</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>51.1790674603175</x:v>
+        <x:v>15.0902777777778</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>5623593</x:v>
+        <x:v>1086410</x:v>
       </x:c>
     </x:row>
     <x:row r="26">
@@ -73430,10 +73430,10 @@
         <x:v>42344</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>56.1433531746032</x:v>
+        <x:v>13.7638888888889</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>6741730</x:v>
+        <x:v>1165690</x:v>
       </x:c>
     </x:row>
     <x:row r="27">
@@ -73444,10 +73444,10 @@
         <x:v>42351</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>59.8611111111111</x:v>
+        <x:v>11.8420138888889</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>6931190</x:v>
+        <x:v>1233900</x:v>
       </x:c>
     </x:row>
     <x:row r="28">
@@ -73458,10 +73458,10 @@
         <x:v>42358</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>51.5973214285714</x:v>
+        <x:v>14.4895833333333</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>7003790</x:v>
+        <x:v>1275630</x:v>
       </x:c>
     </x:row>
     <x:row r="29">
@@ -73472,10 +73472,10 @@
         <x:v>42365</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>40.5321428571429</x:v>
+        <x:v>10.4930555555556</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>7055830</x:v>
+        <x:v>1305850</x:v>
       </x:c>
     </x:row>
     <x:row r="30">
@@ -73486,10 +73486,10 @@
         <x:v>42372</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>61.8167328042328</x:v>
+        <x:v>12.575</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>7214790</x:v>
+        <x:v>1396390</x:v>
       </x:c>
     </x:row>
     <x:row r="31">
@@ -73500,10 +73500,10 @@
         <x:v>42379</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>66.6867063492063</x:v>
+        <x:v>11.3333333333333</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>8431709</x:v>
+        <x:v>1461670</x:v>
       </x:c>
     </x:row>
     <x:row r="32">
@@ -73514,10 +73514,10 @@
         <x:v>42386</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>68.866121031746</x:v>
+        <x:v>9.66840277777778</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>8685179</x:v>
+        <x:v>1517360</x:v>
       </x:c>
     </x:row>
     <x:row r="33">
@@ -73528,10 +73528,10 @@
         <x:v>42393</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>37.8156498015873</x:v>
+        <x:v>7.56979166666667</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>8828056</x:v>
+        <x:v>1560962</x:v>
       </x:c>
     </x:row>
     <x:row r="34">
@@ -73542,10 +73542,10 @@
         <x:v>42407</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>15.3496527777778</x:v>
+        <x:v>2.35108024691358</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>9808341</x:v>
+        <x:v>1560962</x:v>
       </x:c>
     </x:row>
     <x:row r="35">
@@ -73556,10 +73556,10 @@
         <x:v>42414</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>40.0318865740741</x:v>
+        <x:v>9.68287037037037</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>9979781</x:v>
+        <x:v>1602792</x:v>
       </x:c>
     </x:row>
     <x:row r="36">
@@ -73570,10 +73570,10 @@
         <x:v>42421</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>64.3409722222222</x:v>
+        <x:v>10.8420138888889</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>10234601</x:v>
+        <x:v>1665242</x:v>
       </x:c>
     </x:row>
     <x:row r="37">
@@ -73584,10 +73584,10 @@
         <x:v>42428</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>85.6769097222222</x:v>
+        <x:v>13.0034722222222</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>10728100</x:v>
+        <x:v>1740142</x:v>
       </x:c>
     </x:row>
     <x:row r="38">
@@ -73598,10 +73598,10 @@
         <x:v>42435</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>64.4342013888889</x:v>
+        <x:v>11.4930555555556</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>11099241</x:v>
+        <x:v>1806342</x:v>
       </x:c>
     </x:row>
     <x:row r="39">
@@ -73612,10 +73612,10 @@
         <x:v>42442</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>66.5824074074074</x:v>
+        <x:v>12.4884259259259</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>11386877</x:v>
+        <x:v>1860292</x:v>
       </x:c>
     </x:row>
     <x:row r="40">
@@ -73626,10 +73626,10 @@
         <x:v>42449</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>56.3988425925926</x:v>
+        <x:v>10.5185185185185</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>11630520</x:v>
+        <x:v>1905732</x:v>
       </x:c>
     </x:row>
     <x:row r="41">
@@ -73640,10 +73640,10 @@
         <x:v>42456</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>70.6368055555556</x:v>
+        <x:v>12.7916666666667</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>11833954</x:v>
+        <x:v>1942572</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Finished chart section of script
</commit_message>
<xml_diff>
--- a/OpenxmlConsoleApplication/bin/Debug/O&M_Copy.xlsx
+++ b/OpenxmlConsoleApplication/bin/Debug/O&M_Copy.xlsx
@@ -23,7 +23,7 @@
     <x:sheet name="Total Influent" sheetId="16" r:id="rId9"/>
     <x:sheet name="Weekly Inj_Rates" sheetId="8" r:id="rId10"/>
     <x:sheet name="Weekly Ext_Rates" sheetId="9" r:id="rId11"/>
-    <x:sheet name="records" sheetId="17" r:id="Rc6c913541d714057"/>
+    <x:sheet name="records" sheetId="17" r:id="Rfe667684a1bf41fc"/>
   </x:sheets>
   <x:definedNames>
     <x:definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'RAW Data_all'!$A$1:$D$770</x:definedName>
@@ -1932,13 +1932,13 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>('records'!$B$2:$B$41)</c:f>
+              <c:f>('records'!$B$42:$B$79)</c:f>
               <c:numCache/>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('records'!$C$2:$C$41)</c:f>
+              <c:f>('records'!$C$42:$C$79)</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -1966,257 +1966,14 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>('Weekly Inj_Rates'!$H$15,'Weekly Inj_Rates'!$H$34,'Weekly Inj_Rates'!$H$53,'Weekly Inj_Rates'!$H$76,'Weekly Inj_Rates'!$H$91,'Weekly Inj_Rates'!$H$106,'Weekly Inj_Rates'!$H$129,'Weekly Inj_Rates'!$H$144,'Weekly Inj_Rates'!$H$159,'Weekly Inj_Rates'!$H$173,'Weekly Inj_Rates'!$H$184,'Weekly Inj_Rates'!$H$199,'Weekly Inj_Rates'!$H$214,'Weekly Inj_Rates'!$H$225,'Weekly Inj_Rates'!$H$236,'Weekly Inj_Rates'!$H$273,'Weekly Inj_Rates'!$H$288,'Weekly Inj_Rates'!$H$299,'Weekly Inj_Rates'!$H$314,'Weekly Inj_Rates'!$H$329,'Weekly Inj_Rates'!$H$344,'Weekly Inj_Rates'!$H$359,'Weekly Inj_Rates'!$H$370,'Weekly Inj_Rates'!$H$381,'Weekly Inj_Rates'!$H$396,'Weekly Inj_Rates'!$H$411,'Weekly Inj_Rates'!$H$422,'Weekly Inj_Rates'!$H$433,'Weekly Inj_Rates'!$H$457,'Weekly Inj_Rates'!$H$474,'Weekly Inj_Rates'!$H$490,'Weekly Inj_Rates'!$H$502,'Weekly Inj_Rates'!$H$512,'Weekly Inj_Rates'!$H$524,'Weekly Inj_Rates'!$H$540,'Weekly Inj_Rates'!$H$556,'Weekly Inj_Rates'!$H$572,'Weekly Inj_Rates'!$H$584,'Weekly Inj_Rates'!$H$596,'Weekly Inj_Rates'!$H$608)</c:f>
-              <c:numCache>
-                <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="40"/>
-                <c:pt idx="0">
-                  <c:v>42170</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>42177</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>42184</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>42198</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>42205</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>42212</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42219</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>42226</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>42233</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>42240.697916666664</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>42249.337500000001</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>42254.347222222219</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>42261.321527777778</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>42268.665972222225</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>42275.436111111114</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>42279.411805555559</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>42289.338888888888</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>42296.396527777775</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>42303.357638888891</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>42310.379861111112</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>42317.574999999997</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>42324.416666666664</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>42331.348611111112</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>42338.527777777781</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>42345.645833333336</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>42352.334027777775</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>42359.444444444445</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>42366.636805555558</c:v>
-                </c:pt>
-                <c:pt idx="28" formatCode="m/d/yyyy\ h:mm">
-                  <c:v>42373.343055555553</c:v>
-                </c:pt>
-                <c:pt idx="29" formatCode="m/d/yyyy\ h:mm">
-                  <c:v>42380.372916666667</c:v>
-                </c:pt>
-                <c:pt idx="30" formatCode="m/d/yyyy\ h:mm">
-                  <c:v>42387.590277777781</c:v>
-                </c:pt>
-                <c:pt idx="31" formatCode="m/d/yyyy\ h:mm">
-                  <c:v>42394.630555555559</c:v>
-                </c:pt>
-                <c:pt idx="32" formatCode="m/d/yyyy\ h:mm">
-                  <c:v>42412.60833333333</c:v>
-                </c:pt>
-                <c:pt idx="33" formatCode="m/d/yyyy\ h:mm">
-                  <c:v>42416.474999999999</c:v>
-                </c:pt>
-                <c:pt idx="34" formatCode="m/d/yyyy\ h:mm">
-                  <c:v>42422.419444444444</c:v>
-                </c:pt>
-                <c:pt idx="35" formatCode="m/d/yyyy\ h:mm">
-                  <c:v>42429.363888888889</c:v>
-                </c:pt>
-                <c:pt idx="36" formatCode="m/d/yyyy\ h:mm">
-                  <c:v>42436.354166666664</c:v>
-                </c:pt>
-                <c:pt idx="37" formatCode="m/d/yyyy\ h:mm">
-                  <c:v>42443.369444444441</c:v>
-                </c:pt>
-                <c:pt idx="38" formatCode="m/d/yyyy\ h:mm">
-                  <c:v>42450.362500000003</c:v>
-                </c:pt>
-                <c:pt idx="39" formatCode="m/d/yyyy\ h:mm">
-                  <c:v>42457.690972222219</c:v>
-                </c:pt>
-              </c:numCache>
+              <c:f>('records'!$B$2:$B$41)</c:f>
+              <c:numCache/>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('Weekly Ext_Rates'!$G$24,'Weekly Ext_Rates'!$G$43,'Weekly Ext_Rates'!$G$62,'Weekly Ext_Rates'!$G$81,'Weekly Ext_Rates'!$G$96,'Weekly Ext_Rates'!$G$115,'Weekly Ext_Rates'!$G$157,'Weekly Ext_Rates'!$G$182,'Weekly Ext_Rates'!$G$206,'Weekly Ext_Rates'!$G$233,'Weekly Ext_Rates'!$G$252,'Weekly Ext_Rates'!$G$276,'Weekly Ext_Rates'!$G$303,'Weekly Ext_Rates'!$G$322,'Weekly Ext_Rates'!$G$341,'Weekly Ext_Rates'!$G$409,'Weekly Ext_Rates'!$G$436,'Weekly Ext_Rates'!$G$463,'Weekly Ext_Rates'!$G$490,'Weekly Ext_Rates'!$G$517,'Weekly Ext_Rates'!$G$544,'Weekly Ext_Rates'!$G$571,'Weekly Ext_Rates'!$G$590,'Weekly Ext_Rates'!$G$601,'Weekly Ext_Rates'!$G$612,'Weekly Ext_Rates'!$G$623,'Weekly Ext_Rates'!$G$634,'Weekly Ext_Rates'!$G$644,'Weekly Ext_Rates'!$G$687,'Weekly Ext_Rates'!$G$698,'Weekly Ext_Rates'!$G$710,'Weekly Ext_Rates'!$G$722,'Weekly Ext_Rates'!$G$734,'Weekly Ext_Rates'!$G$746,'Weekly Ext_Rates'!$G$758,'Weekly Ext_Rates'!$G$785,'Weekly Ext_Rates'!$G$813,'Weekly Ext_Rates'!$G$833,'Weekly Ext_Rates'!$G$873)</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="39"/>
-                <c:pt idx="0">
-                  <c:v>3.2672697549804566</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.2263865620263061</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>13.681127982651793</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.6592960182840635</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.4426441757008881</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.6015123244620817</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5.0887618369093079</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>18.742774255575259</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>12.003589416226429</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7.9048913157028133</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>14.665558129991911</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12.380763366868639</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>10.387718321125073</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>9.2990869725053749</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>18.221619436565931</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15.848566528659374</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>14.660465558590964</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>8.7491305966567907</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>15.33843097020573</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>14.950672359520716</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>15.335116113330439</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>13.394851398807432</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>15.593622735486486</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>15.085073708190903</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>20.304568932022079</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>19.761578453200041</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>18.12904033767834</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>15.28590107069822</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>16.131771273293516</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>17.981858880299484</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>16.878771198185113</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>9.0415236554635285</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>3.4121827924497659</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.24764791455825383</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>14.447321207159874</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>5.101837591791492</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>6.0475752393821907</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>6.2183426235731378</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>6.183536976732821</c:v>
-                </c:pt>
-              </c:numCache>
+              <c:f>('records'!$C$2:$C$41)</c:f>
+              <c:numCache/>
             </c:numRef>
           </c:val>
           <c:extLst>
@@ -2928,13 +2685,13 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>('records'!$B$2:$B$41)</c:f>
+              <c:f>('records'!$B$42:$B$79)</c:f>
               <c:numCache/>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>('records'!$D$2:$D$41)</c:f>
+              <c:f>('records'!$D$42:$D$79)</c:f>
               <c:numCache/>
             </c:numRef>
           </c:yVal>
@@ -2977,260 +2734,14 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>('Weekly Ext_Rates'!$H$24,'Weekly Ext_Rates'!$H$43,'Weekly Ext_Rates'!$H$62,'Weekly Ext_Rates'!$H$81,'Weekly Ext_Rates'!$H$96,'Weekly Ext_Rates'!$H$115,'Weekly Ext_Rates'!$H$157,'Weekly Ext_Rates'!$H$182,'Weekly Ext_Rates'!$H$206,'Weekly Ext_Rates'!$H$233,'Weekly Ext_Rates'!$H$252,'Weekly Ext_Rates'!$H$276,'Weekly Ext_Rates'!$H$303,'Weekly Ext_Rates'!$H$322,'Weekly Ext_Rates'!$H$341,'Weekly Ext_Rates'!$H$409,'Weekly Ext_Rates'!$H$436,'Weekly Ext_Rates'!$H$463,'Weekly Ext_Rates'!$H$490,'Weekly Ext_Rates'!$H$517,'Weekly Ext_Rates'!$H$544,'Weekly Ext_Rates'!$H$571,'Weekly Ext_Rates'!$H$590,'Weekly Ext_Rates'!$H$601,'Weekly Ext_Rates'!$H$612,'Weekly Ext_Rates'!$H$623,'Weekly Ext_Rates'!$H$634,'Weekly Ext_Rates'!$H$644,'Weekly Ext_Rates'!$H$687,'Weekly Ext_Rates'!$H$698,'Weekly Ext_Rates'!$H$710,'Weekly Ext_Rates'!$H$722,'Weekly Ext_Rates'!$H$734,'Weekly Ext_Rates'!$H$746,'Weekly Ext_Rates'!$H$758,'Weekly Ext_Rates'!$H$785,'Weekly Ext_Rates'!$H$813,'Weekly Ext_Rates'!$H$833,'Weekly Ext_Rates'!$H$853,'Weekly Ext_Rates'!$H$873)</c:f>
-              <c:numCache>
-                <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="40"/>
-                <c:pt idx="0">
-                  <c:v>42170</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>42177</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>42184</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>42198</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>42205</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>42212</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42219</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>42226</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>42233</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>42240.75</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>42249.332638888889</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>42254.318749999999</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>42261.307638888888</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>42268.674305555556</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>42275.4375</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>42279.405555555553</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>42289.323611111111</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>42296.406944444447</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>42303.34097222222</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>42310.34375</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>42317.557638888888</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>42324.413194444445</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>42331.328472222223</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>42338.523611111108</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>42345.631944444445</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>42352.319444444445</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>42359.456250000003</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>42366.652777777781</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>42373.329861111109</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>42380.368055555555</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>42387.585416666669</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>42394.638888888891</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>42412.604166666664</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>42416.525694444441</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>42422.362500000003</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>42431.484027777777</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>42438.374305555553</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>42443.363194444442</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>42450.356944444444</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>42457.697916666664</c:v>
-                </c:pt>
-              </c:numCache>
+              <c:f>('records'!$B$2:$B$41)</c:f>
+              <c:numCache/>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>('Weekly Ext_Rates'!$I$24,'Weekly Ext_Rates'!$I$43,'Weekly Ext_Rates'!$I$62,'Weekly Ext_Rates'!$I$81,'Weekly Ext_Rates'!$I$96,'Weekly Ext_Rates'!$I$115,'Weekly Ext_Rates'!$I$157,'Weekly Ext_Rates'!$I$182,'Weekly Ext_Rates'!$I$206,'Weekly Ext_Rates'!$I$233,'Weekly Ext_Rates'!$I$252,'Weekly Ext_Rates'!$I$276,'Weekly Ext_Rates'!$I$303,'Weekly Ext_Rates'!$I$322,'Weekly Ext_Rates'!$I$341,'Weekly Ext_Rates'!$I$409,'Weekly Ext_Rates'!$I$436,'Weekly Ext_Rates'!$I$463,'Weekly Ext_Rates'!$I$490,'Weekly Ext_Rates'!$I$517,'Weekly Ext_Rates'!$I$544,'Weekly Ext_Rates'!$I$571,'Weekly Ext_Rates'!$I$590,'Weekly Ext_Rates'!$I$601,'Weekly Ext_Rates'!$I$612,'Weekly Ext_Rates'!$I$623,'Weekly Ext_Rates'!$I$634,'Weekly Ext_Rates'!$I$644,'Weekly Ext_Rates'!$I$687,'Weekly Ext_Rates'!$I$698,'Weekly Ext_Rates'!$I$710,'Weekly Ext_Rates'!$I$722,'Weekly Ext_Rates'!$I$734,'Weekly Ext_Rates'!$I$746,'Weekly Ext_Rates'!$I$758,'Weekly Ext_Rates'!$I$785,'Weekly Ext_Rates'!$I$813,'Weekly Ext_Rates'!$I$833,'Weekly Ext_Rates'!$I$853,'Weekly Ext_Rates'!$I$873)</c:f>
-              <c:numCache>
-                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="40"/>
-                <c:pt idx="0">
-                  <c:v>22273.999999999985</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>133659.39999999994</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>209343.39999999997</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>274552.59999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>325636.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>382676.69999999995</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>433876.79999999993</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>561744.39999999991</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>683563.99999999988</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>767860.79999999981</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>915424.99999999988</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1039852.0999999999</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1149129.7999999998</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1213271.5</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1394150.1</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1599458</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1746999.8</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1840336.4</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1991095.4</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2138057.6</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2290935.5</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2423252.2999999998</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2537878</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2651110</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2859099.5999999996</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>3049391.0999999996</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>3235591.7999999993</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>3394088.5999999996</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>3549209.9999999995</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>3731366.0999999996</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>3906784.6999999997</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>3998587.5999999996</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>4086870.1999999997</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>4088268.0999999996</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>4209841.3</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>4449039</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>4569572.7</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>4673767.7</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>4846316.7</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>4955273.7</c:v>
-                </c:pt>
-              </c:numCache>
+              <c:f>('records'!$D$2:$D$41)</c:f>
+              <c:numCache/>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
@@ -73646,6 +73157,538 @@
         <x:v>1942572</x:v>
       </x:c>
     </x:row>
+    <x:row r="42">
+      <x:c t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42169</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>1.509375</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>10754</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43">
+      <x:c t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42176</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>15.4479166666667</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>55244</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44">
+      <x:c t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42183</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>14.6232638888889</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>139474</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45">
+      <x:c t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42197</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>4.94965277777778</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>167984</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46">
+      <x:c t="n">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42204</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>10.1930555555556</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>241374</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47">
+      <x:c t="n">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42211</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>10.0694444444444</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>299374</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48">
+      <x:c t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42218</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>4.22395833333333</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>323704</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49">
+      <x:c t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42225</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>10.6684027777778</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>385154</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50">
+      <x:c t="n">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42232</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>7.01041666666667</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>425534</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51">
+      <x:c t="n">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42239</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>6.41840277777778</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>462504</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="52">
+      <x:c t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42246</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>11.8194444444444</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>496544</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="53">
+      <x:c t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42253</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>12.796875</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>570254</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="54">
+      <x:c t="n">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42260</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>12.0520833333333</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>639674</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="55">
+      <x:c t="n">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42267</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>8.51041666666667</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>664184</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="56">
+      <x:c t="n">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42274</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>8.00868055555556</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>710314</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="57">
+      <x:c t="n">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42281</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>10.6979166666667</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>771934</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="58">
+      <x:c t="n">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42288</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>10.3472222222222</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>831534</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="59">
+      <x:c t="n">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42295</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>11.0954861111111</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>895444</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="60">
+      <x:c t="n">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42302</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>11.8229166666667</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>963544</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="61">
+      <x:c t="n">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42309</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>10.3611111111111</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>1023224</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="62">
+      <x:c t="n">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42316</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>11.4409722222222</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>1089124</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="63">
+      <x:c t="n">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42323</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>21.6979166666667</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>1214104</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="64">
+      <x:c t="n">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42330</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>10.9270833333333</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>1245574</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="65">
+      <x:c t="n">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42337</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>7.19444444444444</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>1287014</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="66">
+      <x:c t="n">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42344</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>10.8333333333333</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>1349414</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="67">
+      <x:c t="n">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42351</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>10.5538194444444</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>1410204</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="68">
+      <x:c t="n">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42372</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>9.44907407407407</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>1410204</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="69">
+      <x:c t="n">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42379</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>11.375</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>1475724</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="70">
+      <x:c t="n">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42386</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>11.5972222222222</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>1542524</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="71">
+      <x:c t="n">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42393</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>5.76909722222222</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>1575754</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="72">
+      <x:c t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42407</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>3.0516975308642</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>1575754</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="73">
+      <x:c t="n">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42414</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>10.0138888888889</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>1619014</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="74">
+      <x:c t="n">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42421</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>11.2222222222222</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>1683654</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="75">
+      <x:c t="n">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42428</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>28.7013888888889</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>1848974</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="76">
+      <x:c t="n">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42435</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>11.9767361111111</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>1917960</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="77">
+      <x:c t="n">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42442</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>12.1203703703704</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>1970320</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="78">
+      <x:c t="n">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42449</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>10.224537037037</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>2014490</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="79">
+      <x:c t="n">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c s="5">
+        <x:v>42456</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>12.4166666666667</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>2050250</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed Quarter Record Parser
</commit_message>
<xml_diff>
--- a/OpenxmlConsoleApplication/bin/Debug/O&M_Copy.xlsx
+++ b/OpenxmlConsoleApplication/bin/Debug/O&M_Copy.xlsx
@@ -15,8 +15,8 @@
     <x:sheet name="RAW Data_all" sheetId="2" r:id="rId1"/>
     <x:sheet name="WeeklyFlowRates" sheetId="3" r:id="rId2"/>
     <x:sheet name="SumVol" sheetId="4" r:id="rId3"/>
-    <x:sheet name="records" sheetId="5" r:id="R42cf51d157f64cc2"/>
-    <x:sheet name="stationReport" sheetId="6" r:id="R9316e4d9be4d441e"/>
+    <x:sheet name="records" sheetId="5" r:id="R73cb72d5be884f22"/>
+    <x:sheet name="stationReport" sheetId="6" r:id="R92f4c33a20a54470"/>
   </x:sheets>
   <x:externalReferences>
     <x:externalReference r:id="rId4"/>
@@ -1412,7 +1412,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('records'!$E$3:$E$42)</c:f>
+              <c:f>('records'!$G$3:$G$42)</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -1446,7 +1446,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('records'!$E$43:$E$82)</c:f>
+              <c:f>('records'!$G$43:$G$82)</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -27550,7 +27550,7 @@
         <x:v>1.58094968821967</x:v>
       </x:c>
       <x:c r="H3" s="293" t="n">
-        <x:v>3.79985683607731</x:v>
+        <x:v>7.9335329286223</x:v>
       </x:c>
     </x:row>
     <x:row r="4">
@@ -27867,7 +27867,7 @@
         <x:v>10.8869367465983</x:v>
       </x:c>
       <x:c r="H18" s="293" t="n">
-        <x:v>4.2151034980039</x:v>
+        <x:v>9.24385631173491</x:v>
       </x:c>
     </x:row>
     <x:row r="19">
@@ -28142,7 +28142,7 @@
         <x:v>9.21208084898285</x:v>
       </x:c>
       <x:c r="H31" s="293" t="n">
-        <x:v>3.92580664721775</x:v>
+        <x:v>8.72714609836619</x:v>
       </x:c>
     </x:row>
     <x:row r="32">

</xml_diff>